<commit_message>
VISTA-5536: - Updated some Amenity and Building Types - Deleted no-repeat randomly preloaded entities regarding the number of elements to create to avoid problem when creating thousands of items (load testiong, etc)
</commit_message>
<xml_diff>
--- a/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/util/building-amenities.xlsx
+++ b/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/util/building-amenities.xlsx
@@ -125,7 +125,7 @@
     <t>Extra large storage unit</t>
   </si>
   <si>
-    <t>furnishedUnitsAvailable</t>
+    <t>furnishedUnits</t>
   </si>
   <si>
     <t>Furnished Units Available</t>
@@ -134,7 +134,7 @@
     <t>Beautiful Furnished Suite</t>
   </si>
   <si>
-    <t>intrusionAlarmAvailable</t>
+    <t>intrusionAlarm</t>
   </si>
   <si>
     <t>Intrusion Alarm Available</t>
@@ -284,8 +284,8 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>